<commit_message>
Updates to Script / Module 7
</commit_message>
<xml_diff>
--- a/Scraper_output/Case_status_by_year_2018-11-14 17:36:52.240067.xlsx
+++ b/Scraper_output/Case_status_by_year_2018-11-14 17:36:52.240067.xlsx
@@ -65,7 +65,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -95,6 +95,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -164,7 +169,334 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB3B3B3"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF004586"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <c:chart>
+    <c:plotArea>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Percent_Dismissed</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2017</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$E$2:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.58</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.57</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.57</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.56</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.62</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="64581490"/>
+        <c:axId val="51699300"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="64581490"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="51699300"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="51699300"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:latin typeface="Arial"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="64581490"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:latin typeface="Arial"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>34560</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>38160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>80640</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>162000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="4738320" y="38160"/>
+        <a:ext cx="7634520" cy="4886280"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -175,7 +507,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="topLeft" activeCell="Q19" activeCellId="0" sqref="Q19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -343,5 +675,6 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>